<commit_message>
Save sheet data through XmlWriter 15/18 - Add ability to load and save charset and a scheme. Scheme has been added to the public API.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Styles/UsingRichText.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Styles/UsingRichText.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
     <x:r>
       <x:rPr>
@@ -172,6 +172,60 @@
         <x:family val="2"/>
       </x:rPr>
       <x:t>with a gray background</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="25"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Arial"/>
+        <x:family val="2"/>
+        <x:scheme val="major"/>
+      </x:rPr>
+      <x:t>Major scheme</x:t>
+    </x:r>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="25"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t xml:space="preserve"> </x:t>
+    </x:r>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="25"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Times New Roman"/>
+        <x:family val="2"/>
+        <x:scheme val="minor"/>
+      </x:rPr>
+      <x:t>Minor scheme</x:t>
+    </x:r>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="25"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t xml:space="preserve"> </x:t>
+    </x:r>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="25"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Cambria"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>No scheme</x:t>
     </x:r>
   </x:si>
 </x:sst>
@@ -182,7 +236,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="2">
+  <x:fonts count="3">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -194,6 +248,13 @@
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF0000FF"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="25"/>
+      <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
       <x:family val="2"/>
     </x:font>
@@ -230,7 +291,7 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="3">
+  <x:cellStyleXfs count="4">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -240,8 +301,11 @@
     <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="3">
+  <x:cellXfs count="4">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -251,6 +315,10 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -549,13 +617,14 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B5"/>
+  <x:dimension ref="A1:B6"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="2" width="34.970625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="81.860625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="34.970625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:2">
@@ -579,6 +648,11 @@
         <x:v>4</x:v>
       </x:c>
     </x:row>
+    <x:row r="6" spans="1:2">
+      <x:c r="A6" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Replace saving mechanism of shared string table with a more straightforward mechanism of just writing the relevant entries from SharedStringTable. It's faster (no need to traverse whole workbook).
Test fiels had to be changed due to different order of entries (pivot tables) and the UsingRichText had same rich text twice.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Styles/UsingRichText.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Styles/UsingRichText.xlsx
@@ -48,62 +48,6 @@
     </x:r>
   </x:si>
   <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="11"/>
-        <x:color rgb="FFFF0000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>Hell</x:t>
-    </x:r>
-    <x:r>
-      <x:rPr>
-        <x:u val="single"/>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="11"/>
-        <x:color rgb="FFFF0000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>o</x:t>
-    </x:r>
-    <x:r>
-      <x:rPr>
-        <x:b/>
-        <x:u val="single"/>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="11"/>
-        <x:color rgb="FF0000FF"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t xml:space="preserve"> BIG </x:t>
-    </x:r>
-    <x:r>
-      <x:rPr>
-        <x:u val="single"/>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="11"/>
-        <x:color rgb="FFFF0000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>W</x:t>
-    </x:r>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="11"/>
-        <x:color rgb="FFFF0000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>orld</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
     <x:t>" BIG " is Bold.</x:t>
   </x:si>
   <x:si>
@@ -111,33 +55,55 @@
       <x:rPr>
         <x:vertAlign val="baseline"/>
         <x:sz val="11"/>
-        <x:color rgb="FF008000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>Some</x:t>
+        <x:color rgb="FFFF0000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>Hell</x:t>
+    </x:r>
+    <x:r>
+      <x:rPr>
+        <x:u val="single"/>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="11"/>
+        <x:color rgb="FFFF0000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>o</x:t>
     </x:r>
     <x:r>
       <x:rPr>
         <x:b/>
+        <x:u val="single"/>
         <x:vertAlign val="baseline"/>
         <x:sz val="11"/>
         <x:color rgb="FF0000FF"/>
         <x:rFont val="Calibri"/>
         <x:family val="2"/>
       </x:rPr>
-      <x:t xml:space="preserve"> rich text </x:t>
-    </x:r>
-    <x:r>
-      <x:rPr>
-        <x:i/>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="11"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>with a gray background</x:t>
+      <x:t xml:space="preserve"> BIG </x:t>
+    </x:r>
+    <x:r>
+      <x:rPr>
+        <x:u val="single"/>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="11"/>
+        <x:color rgb="FFFF0000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>W</x:t>
+    </x:r>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="11"/>
+        <x:color rgb="FFFF0000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>orld</x:t>
     </x:r>
   </x:si>
   <x:si>
@@ -634,10 +600,10 @@
     </x:row>
     <x:row r="3" spans="1:2">
       <x:c r="A3" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:2">
@@ -645,12 +611,12 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
       <x:c r="A6" s="3" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>